<commit_message>
add chart to index
</commit_message>
<xml_diff>
--- a/customer/format.xlsx
+++ b/customer/format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\project\project_uts\customer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E55F741-BBA2-4553-944E-82B71833CFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9D7728-80E9-4B8D-B26C-49C6A579DD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="1170" windowWidth="17250" windowHeight="8850" xr2:uid="{A4DDEF5A-87B1-4B32-825E-D8F9826ABF07}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A4DDEF5A-87B1-4B32-825E-D8F9826ABF07}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Customer Name</t>
   </si>
@@ -48,40 +48,10 @@
     <t>Ad</t>
   </si>
   <si>
-    <t>Alex</t>
+    <t>test</t>
   </si>
   <si>
-    <t>PIK</t>
-  </si>
-  <si>
-    <t>Cahaya Tirta</t>
-  </si>
-  <si>
-    <t>Nur Cahya</t>
-  </si>
-  <si>
-    <t>Kusuma Eka</t>
-  </si>
-  <si>
-    <t>Mega Tri</t>
-  </si>
-  <si>
-    <t>Purnama Mega</t>
-  </si>
-  <si>
-    <t>Bandung</t>
-  </si>
-  <si>
-    <t>Semarang</t>
-  </si>
-  <si>
-    <t>Jakarta</t>
-  </si>
-  <si>
-    <t>Depok</t>
-  </si>
-  <si>
-    <t>Bekasi</t>
+    <t>Bogor</t>
   </si>
 </sst>
 </file>
@@ -470,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CA564A-5E29-49E0-B9B6-FCA3184BDD20}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,81 +474,26 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>129129128</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>129129128</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>129129128</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>129129128</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>129129128</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>129129128</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
+      <c r="A7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>